<commit_message>
Commit changed pom 2
</commit_message>
<xml_diff>
--- a/Display_Bookshelves/StudyChairsDetails.xlsx
+++ b/Display_Bookshelves/StudyChairsDetails.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -86,15 +86,15 @@
     <t>₹16,999 ₹13,599</t>
   </si>
   <si>
+    <t>(Ash Grey)</t>
+  </si>
+  <si>
+    <t>₹10,999 ₹8,799</t>
+  </si>
+  <si>
     <t>(Carbon Black)</t>
   </si>
   <si>
-    <t>(Ash Grey)</t>
-  </si>
-  <si>
-    <t>₹10,999 ₹8,799</t>
-  </si>
-  <si>
     <t>Mika Study Chair</t>
   </si>
   <si>
@@ -131,6 +131,12 @@
     <t>₹10,999</t>
   </si>
   <si>
+    <t>Axis Folding Chair</t>
+  </si>
+  <si>
+    <t>₹4,999</t>
+  </si>
+  <si>
     <t>Poulain Accent Chair</t>
   </si>
   <si>
@@ -140,12 +146,45 @@
     <t>(Two Tone, Fabric Seat)</t>
   </si>
   <si>
+    <t>Doris Swivel Accent Chair</t>
+  </si>
+  <si>
+    <t>(White, Leatherette Material)</t>
+  </si>
+  <si>
+    <t>₹8,699</t>
+  </si>
+  <si>
+    <t>(Blue, Fabric Material)</t>
+  </si>
+  <si>
+    <t>(Dark Grey, Fabric Material)</t>
+  </si>
+  <si>
     <t>Dorsey Study Chair</t>
   </si>
   <si>
     <t>₹5,499 ₹4,124</t>
   </si>
   <si>
+    <t>Hawley Study Chair</t>
+  </si>
+  <si>
+    <t>(Mahogany Finish)</t>
+  </si>
+  <si>
+    <t>₹6,999</t>
+  </si>
+  <si>
+    <t>₹6,999 ₹5,949</t>
+  </si>
+  <si>
+    <t>(Scarlet Red)</t>
+  </si>
+  <si>
+    <t>₹13,599 ₹11,559</t>
+  </si>
+  <si>
     <t>Galen Study Chair</t>
   </si>
   <si>
@@ -155,28 +194,10 @@
     <t>₹10,999 ₹7,699</t>
   </si>
   <si>
-    <t>Hawley Study Chair</t>
-  </si>
-  <si>
-    <t>(Mahogany Finish)</t>
-  </si>
-  <si>
-    <t>₹6,999</t>
-  </si>
-  <si>
-    <t>₹6,999 ₹5,949</t>
-  </si>
-  <si>
     <t>Cohen Study Chair</t>
   </si>
   <si>
     <t>₹8,499 ₹6,374</t>
-  </si>
-  <si>
-    <t>(Scarlet Red)</t>
-  </si>
-  <si>
-    <t>₹13,599 ₹11,559</t>
   </si>
   <si>
     <t>Barry Study Chair</t>
@@ -230,7 +251,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -343,7 +364,7 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -351,10 +372,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -406,18 +427,18 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -425,13 +446,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
@@ -447,57 +468,101 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
         <v>53</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C25" t="s">
         <v>56</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
         <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>